<commit_message>
Modified headers to include namespace separator for compatibility with pivot tables.
</commit_message>
<xml_diff>
--- a/ClearbitEnrichmentToExcel/ClearbitEnrichmentToExcel/bin/Debug/Cust_Data.xlsx
+++ b/ClearbitEnrichmentToExcel/ClearbitEnrichmentToExcel/bin/Debug/Cust_Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="328">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -21,13 +21,13 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">fullName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">givenName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">familyName</t>
+    <t xml:space="preserve">name.fullName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name.givenName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name.familyName</t>
   </si>
   <si>
     <t xml:space="preserve">email</t>
@@ -48,25 +48,25 @@
     <t xml:space="preserve">geo</t>
   </si>
   <si>
-    <t xml:space="preserve">city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">state</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stateCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">countryCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lng</t>
+    <t xml:space="preserve">geo.city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.stateCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.countryCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.lng</t>
   </si>
   <si>
     <t xml:space="preserve">bio</t>
@@ -81,435 +81,507 @@
     <t xml:space="preserve">employment</t>
   </si>
   <si>
+    <t xml:space="preserve">employment.domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employment.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employment.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employment.role</t>
+  </si>
+  <si>
+    <t xml:space="preserve">employment.seniority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facebook.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.blog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.followers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.following</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.followers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.following</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.statuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.favorites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">twitter.avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkedin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">linkedin.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">googleplus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">googleplus.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aboutme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aboutme.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aboutme.bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aboutme.avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.urls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.urls.value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.urls.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.avatar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.avatars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.avatars.url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gravatar.avatars.type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuzzy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailProvider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexedAt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">247193a9-33a1-4cc8-a997-9af62dd8da61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex MacCaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MacCaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alex@alexmaccaw.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Francisco, CA, US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">America/Los_Angeles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Francisco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.7749295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-122.4194155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@clearbit co-founder. Tea, Earl Grey, hot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://alexmaccaw.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/247193a9-33a1-4cc8-a997-9af62dd8da61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alexmaccaw.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">founder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">executive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amaccaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maccman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://avatars1.githubusercontent.com/u/2142?v=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clearbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3419</t>
+  </si>
+  <si>
+    <t xml:space="preserve">101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maccaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2006261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18450</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pbs.twimg.com/profile_images/658880981017882629/nlXSOJnc.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in/alex-maccaw-ab592978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Software engineer &amp; traveller. Walker, skier, reader, tennis player, breather, ginger beer drinker, scooterer &amp; generally enjoying things :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personal Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://2.gravatar.com/avatar/994909da96d3afaf4daaf54973914b64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thumbnail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/30/2017 5:41:04 AM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5c180767-8095-495e-928b-677895ba1cfc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lachy Groom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lachy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Groom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lachy@stripe.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I work on International @stripe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://lachygroom.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/5c180767-8095-495e-928b-677895ba1cfc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stripe.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stripe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cards Lead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lachygroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14647871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pbs.twimg.com/profile_images/2823877912/383da5c4764bfe64442738a03171eeaa.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in/lachy-groom-b218895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lachy2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://1.gravatar.com/avatar/b683590be3a1236b315614d623349454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/20/2017 12:51:24 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2be91c0-b6a0-4615-bfd8-a9e0a018e390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harlow Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harlow@clearbit.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Developer at @Clearbit by way of @HotelTonight and @thoughtbot. I like fast APIs, streaming event data, and of course my lovely @tayloresque.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/harlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/a2be91c0-b6a0-4615-bfd8-a9e0a018e390</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clearbit.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">developer and co-founder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">739782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://avatars.githubusercontent.com/u/739782?v=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://hward.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harlow_ward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">192721786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">San Francisco, CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pbs.twimg.com/profile_images/758780748870541313/ossNObOE.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in/harlowward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hrwiv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://0.gravatar.com/avatar/036299c03c161f673ddef75721835a04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/9/2017 11:24:13 PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">legalName</t>
+  </si>
+  <si>
     <t xml:space="preserve">domain</t>
   </si>
   <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">role</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seniority</t>
-  </si>
-  <si>
-    <t xml:space="preserve">facebook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">handle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">github</t>
-  </si>
-  <si>
-    <t xml:space="preserve">company</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">followers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">following</t>
-  </si>
-  <si>
-    <t xml:space="preserve">twitter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">statuses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">favorites</t>
-  </si>
-  <si>
-    <t xml:space="preserve">linkedin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">googleplus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aboutme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gravatar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">urls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">avatars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">url</t>
+    <t xml:space="preserve">domainAliases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.h1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.metaDescription</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.metaAuthor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.phoneNumbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">site.emailAddresses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category.sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category.industryGroup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category.industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category.subIndustry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foundedYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.streetNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.streetName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.subPremise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geo.postalCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facebook.likes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crunchbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crunchbase.handle</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
-    <t xml:space="preserve">fuzzy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailProvider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indexedAt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">247193a9-33a1-4cc8-a997-9af62dd8da61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex MacCaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MacCaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alex@alexmaccaw.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Francisco, CA, US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">America/Los_Angeles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Francisco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">California</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.7749295</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-122.4194155</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@clearbit co-founder. Tea, Earl Grey, hot.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://alexmaccaw.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/247193a9-33a1-4cc8-a997-9af62dd8da61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alexmaccaw.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">founder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">executive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amaccaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maccman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://avatars1.githubusercontent.com/u/2142?v=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clearbit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3419</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maccaw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2006261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18450</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9787</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5997</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://pbs.twimg.com/profile_images/658880981017882629/nlXSOJnc.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in/alex-maccaw-ab592978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software engineer &amp; traveller. Walker, skier, reader, tennis player, breather, ginger beer drinker, scooterer &amp; generally enjoying things :)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personal Website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://2.gravatar.com/avatar/994909da96d3afaf4daaf54973914b64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">thumbnail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">False</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/30/2017 5:41:04 AM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5c180767-8095-495e-928b-677895ba1cfc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lachy Groom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lachy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lachy@stripe.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I work on International @stripe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://lachygroom.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/5c180767-8095-495e-928b-677895ba1cfc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stripe.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stripe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cards Lead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lachygroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14647871</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">326</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13178</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1552</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://pbs.twimg.com/profile_images/2823877912/383da5c4764bfe64442738a03171eeaa.jpeg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in/lachy-groom-b218895</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lachy2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://1.gravatar.com/avatar/b683590be3a1236b315614d623349454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/20/2017 12:51:24 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a2be91c0-b6a0-4615-bfd8-a9e0a018e390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harlow Ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harlow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harlow@clearbit.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Developer at @Clearbit by way of @HotelTonight and @thoughtbot. I like fast APIs, streaming event data, and of course my lovely @tayloresque.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/harlow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://d1ts43dypk8bqh.cloudfront.net/v1/avatars/a2be91c0-b6a0-4615-bfd8-a9e0a018e390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clearbit.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">developer and co-founder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harlow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">739782</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://avatars.githubusercontent.com/u/739782?v=3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://hward.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harlow_ward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">192721786</t>
-  </si>
-  <si>
-    <t xml:space="preserve">632</t>
-  </si>
-  <si>
-    <t xml:space="preserve">291</t>
-  </si>
-  <si>
-    <t xml:space="preserve">493</t>
-  </si>
-  <si>
-    <t xml:space="preserve">999</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Francisco, CA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://pbs.twimg.com/profile_images/758780748870541313/ossNObOE.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in/harlowward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hrwiv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://0.gravatar.com/avatar/036299c03c161f673ddef75721835a04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/9/2017 11:24:13 PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">legalName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">domainAliases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metaDescription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">metaAuthor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phoneNumbers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailAddresses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">industryGroup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subIndustry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foundedYear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">streetNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">streetName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">subPremise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">postalCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">likes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crunchbase</t>
-  </si>
-  <si>
     <t xml:space="preserve">ticker</t>
   </si>
   <si>
@@ -519,28 +591,28 @@
     <t xml:space="preserve">metrics</t>
   </si>
   <si>
-    <t xml:space="preserve">alexaUsRank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alexaGlobalRank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">googleRank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">employeesRange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">marketCap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raised</t>
-  </si>
-  <si>
-    <t xml:space="preserve">annualRevenue</t>
+    <t xml:space="preserve">metrics.alexaUsRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.alexaGlobalRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.googleRank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.employeesRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.marketCap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.raised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metrics.annualRevenue</t>
   </si>
   <si>
     <t xml:space="preserve">tech</t>
@@ -1045,390 +1117,390 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AD1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AF1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="AG1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="AH1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AI1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AJ1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AK1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AM1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="AN1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="AO1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="AP1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="AQ1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="AR1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="AS1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="AT1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="AU1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="AV1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="AW1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="AX1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="AY1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="AZ1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="BA1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="BB1" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="BC1" t="s">
-        <v>18</v>
+        <v>54</v>
       </c>
       <c r="BD1" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="BE1" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="BF1" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="BG1" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="BH1" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="BI1" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="BJ1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="BK1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="BL1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="BM1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="BN1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="BO1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="BP1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G2"/>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="J2" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K2"/>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="N2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="P2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="Q2" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="R2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="T2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="U2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="V2"/>
       <c r="W2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="X2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="Y2" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="Z2" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="AA2" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="AB2"/>
       <c r="AC2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="AD2"/>
       <c r="AE2" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="AF2" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="AG2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="AH2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="AI2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="AJ2" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="AK2" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="AL2"/>
       <c r="AM2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AT2" t="s">
         <v>76</v>
       </c>
-      <c r="AN2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>56</v>
-      </c>
       <c r="AU2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="AV2" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="AW2"/>
       <c r="AX2" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="BC2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="BD2"/>
       <c r="BE2"/>
       <c r="BF2" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="BG2"/>
       <c r="BH2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="BI2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="BJ2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="BK2"/>
       <c r="BL2" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="BM2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="BN2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BO2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BP2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K3"/>
       <c r="L3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="M3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="P3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="R3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="T3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="U3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="V3"/>
       <c r="W3" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="X3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="Y3" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="Z3"/>
       <c r="AA3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="AB3"/>
       <c r="AC3"/>
@@ -1442,38 +1514,38 @@
       <c r="AK3"/>
       <c r="AL3"/>
       <c r="AM3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="AN3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="AO3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="AP3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="AQ3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="AR3" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="AS3" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="AT3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="AU3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="AV3" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="AW3"/>
       <c r="AX3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="AY3"/>
       <c r="AZ3"/>
@@ -1483,165 +1555,165 @@
       <c r="BD3"/>
       <c r="BE3"/>
       <c r="BF3" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="BG3"/>
       <c r="BH3"/>
       <c r="BI3"/>
       <c r="BJ3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="BK3"/>
       <c r="BL3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="BM3" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="BN3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BO3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BP3" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" t="s">
         <v>115</v>
       </c>
-      <c r="D4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
-      </c>
       <c r="H4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="J4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="K4"/>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="R4" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="S4" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="T4" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="U4" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="V4"/>
       <c r="W4" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="X4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="Y4" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="Z4" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="AA4" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="AB4"/>
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="AF4" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="AG4" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="AH4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="AI4" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="AJ4" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="AK4" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="AL4"/>
       <c r="AM4" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="AN4" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="AO4" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="AP4" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="AQ4" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="AR4" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="AS4" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="AT4" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="AU4" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="AV4" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="AW4"/>
       <c r="AX4" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="AY4"/>
       <c r="AZ4"/>
@@ -1651,29 +1723,29 @@
       <c r="BD4"/>
       <c r="BE4"/>
       <c r="BF4" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="BG4"/>
       <c r="BH4"/>
       <c r="BI4"/>
       <c r="BJ4" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="BK4"/>
       <c r="BL4" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="BM4" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="BN4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BO4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BP4" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1697,75 +1769,109 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
       <c r="E1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
-      <c r="K1"/>
-      <c r="L1"/>
-      <c r="M1"/>
+        <v>165</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" t="s">
+        <v>165</v>
+      </c>
+      <c r="K1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>165</v>
+      </c>
       <c r="N1" t="s">
         <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>166</v>
       </c>
       <c r="P1" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="Q1" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="R1" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="S1" t="s">
-        <v>148</v>
-      </c>
-      <c r="T1"/>
+        <v>170</v>
+      </c>
+      <c r="T1" t="s">
+        <v>170</v>
+      </c>
       <c r="U1" t="s">
-        <v>149</v>
-      </c>
-      <c r="V1"/>
-      <c r="W1"/>
-      <c r="X1"/>
-      <c r="Y1"/>
+        <v>171</v>
+      </c>
+      <c r="V1" t="s">
+        <v>171</v>
+      </c>
+      <c r="W1" t="s">
+        <v>171</v>
+      </c>
+      <c r="X1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>171</v>
+      </c>
       <c r="Z1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="AA1" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="AB1" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="AC1" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="AD1" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="AE1" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF1"/>
-      <c r="AG1"/>
-      <c r="AH1"/>
-      <c r="AI1"/>
+        <v>177</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>177</v>
+      </c>
       <c r="AJ1" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="AK1" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="AL1" t="s">
         <v>7</v>
@@ -1780,19 +1886,19 @@
         <v>10</v>
       </c>
       <c r="AP1" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="AQ1" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="AR1" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="AS1" t="s">
         <v>11</v>
       </c>
       <c r="AT1" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="AU1" t="s">
         <v>12</v>
@@ -1813,141 +1919,193 @@
         <v>17</v>
       </c>
       <c r="BA1" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="BB1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="BC1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="BD1" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="BE1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="BF1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="BG1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="BH1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="BI1" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="BJ1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="BK1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="BL1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="BM1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="BN1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="BO1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="BP1" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="BQ1" t="s">
-        <v>27</v>
+        <v>187</v>
       </c>
       <c r="BR1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="BS1" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="BT1" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="BU1" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="BV1" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="BW1" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="BX1" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="BY1" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="BZ1" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="CA1" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="CB1" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="CC1" t="s">
-        <v>174</v>
+        <v>198</v>
       </c>
       <c r="CD1" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="CE1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="CF1" t="s">
-        <v>176</v>
-      </c>
-      <c r="CG1"/>
-      <c r="CH1"/>
-      <c r="CI1"/>
-      <c r="CJ1"/>
-      <c r="CK1"/>
-      <c r="CL1"/>
-      <c r="CM1"/>
-      <c r="CN1"/>
-      <c r="CO1"/>
-      <c r="CP1"/>
-      <c r="CQ1"/>
-      <c r="CR1"/>
-      <c r="CS1"/>
-      <c r="CT1"/>
-      <c r="CU1"/>
+        <v>200</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CS1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CT1" t="s">
+        <v>200</v>
+      </c>
+      <c r="CU1" t="s">
+        <v>200</v>
+      </c>
       <c r="CV1" t="s">
-        <v>177</v>
-      </c>
-      <c r="CW1"/>
-      <c r="CX1"/>
-      <c r="CY1"/>
-      <c r="CZ1"/>
-      <c r="DA1"/>
-      <c r="DB1"/>
-      <c r="DC1"/>
-      <c r="DD1"/>
-      <c r="DE1"/>
-      <c r="DF1"/>
-      <c r="DG1"/>
+        <v>201</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>201</v>
+      </c>
+      <c r="CZ1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DC1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DD1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DE1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DF1" t="s">
+        <v>201</v>
+      </c>
+      <c r="DG1" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="E2"/>
       <c r="F2"/>
@@ -1960,22 +2118,22 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="P2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="R2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="S2"/>
       <c r="T2"/>
       <c r="U2"/>
       <c r="V2" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="W2"/>
       <c r="X2"/>
@@ -1987,15 +2145,15 @@
       <c r="AD2"/>
       <c r="AE2"/>
       <c r="AF2" t="s">
-        <v>180</v>
+        <v>204</v>
       </c>
       <c r="AG2" t="s">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="AH2"/>
       <c r="AI2"/>
       <c r="AJ2" t="s">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="AK2"/>
       <c r="AL2"/>
@@ -2014,7 +2172,7 @@
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="BB2"/>
       <c r="BC2"/>
@@ -2023,43 +2181,43 @@
       <c r="BF2"/>
       <c r="BG2"/>
       <c r="BH2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>207</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>208</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BM2" t="s">
         <v>76</v>
       </c>
-      <c r="BI2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>183</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>184</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>56</v>
-      </c>
       <c r="BN2" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="BO2" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="BP2"/>
       <c r="BQ2"/>
       <c r="BR2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BS2" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="BT2"/>
       <c r="BU2"/>
       <c r="BV2"/>
       <c r="BW2"/>
       <c r="BX2" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="BY2"/>
       <c r="BZ2"/>
@@ -2068,20 +2226,20 @@
       <c r="CC2"/>
       <c r="CD2"/>
       <c r="CE2" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="CF2"/>
       <c r="CG2" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="CH2" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="CI2" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="CJ2" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="CK2"/>
       <c r="CL2"/>
@@ -2096,7 +2254,7 @@
       <c r="CU2"/>
       <c r="CV2"/>
       <c r="CW2" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="CX2"/>
       <c r="CY2"/>
@@ -2111,228 +2269,228 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>219</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="E3"/>
       <c r="F3" t="s">
-        <v>197</v>
+        <v>221</v>
       </c>
       <c r="G3" t="s">
-        <v>198</v>
+        <v>222</v>
       </c>
       <c r="H3" t="s">
-        <v>199</v>
+        <v>223</v>
       </c>
       <c r="I3" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="J3" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="K3" t="s">
-        <v>202</v>
+        <v>226</v>
       </c>
       <c r="L3" t="s">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="M3" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="N3"/>
       <c r="O3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="P3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="Q3" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="R3"/>
       <c r="S3"/>
       <c r="T3"/>
       <c r="U3"/>
       <c r="V3" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="W3" t="s">
-        <v>207</v>
+        <v>231</v>
       </c>
       <c r="X3" t="s">
-        <v>208</v>
+        <v>232</v>
       </c>
       <c r="Y3" t="s">
-        <v>209</v>
+        <v>233</v>
       </c>
       <c r="Z3"/>
       <c r="AA3" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="AB3" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="AC3" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="AD3" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="AE3"/>
       <c r="AF3" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="AG3" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="AH3" t="s">
-        <v>215</v>
+        <v>239</v>
       </c>
       <c r="AI3"/>
       <c r="AJ3" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="AK3" t="s">
-        <v>216</v>
+        <v>240</v>
       </c>
       <c r="AL3" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="AM3" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="AN3" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="AO3"/>
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3"/>
       <c r="AS3" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="AT3"/>
       <c r="AU3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AV3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="AW3" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="AX3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AY3" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="AZ3" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="BA3" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="BB3"/>
       <c r="BC3" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="BD3"/>
       <c r="BE3"/>
       <c r="BF3" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="BG3"/>
       <c r="BH3" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="BI3" t="s">
-        <v>222</v>
+        <v>246</v>
       </c>
       <c r="BJ3" t="s">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="BK3" t="s">
-        <v>224</v>
+        <v>248</v>
       </c>
       <c r="BL3" t="s">
-        <v>225</v>
+        <v>249</v>
       </c>
       <c r="BM3" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="BN3" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
       <c r="BO3" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="BP3"/>
       <c r="BQ3" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="BR3" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BS3" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="BT3"/>
       <c r="BU3"/>
       <c r="BV3"/>
       <c r="BW3" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="BX3" t="s">
-        <v>230</v>
+        <v>254</v>
       </c>
       <c r="BY3"/>
       <c r="BZ3" t="s">
-        <v>231</v>
+        <v>255</v>
       </c>
       <c r="CA3" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="CB3"/>
       <c r="CC3" t="s">
-        <v>233</v>
+        <v>257</v>
       </c>
       <c r="CD3"/>
       <c r="CE3" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
       <c r="CF3"/>
       <c r="CG3" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
       <c r="CH3" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="CI3" t="s">
-        <v>221</v>
+        <v>245</v>
       </c>
       <c r="CJ3" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="CK3" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="CL3" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="CM3" t="s">
-        <v>240</v>
+        <v>264</v>
       </c>
       <c r="CN3" t="s">
-        <v>241</v>
+        <v>265</v>
       </c>
       <c r="CO3"/>
       <c r="CP3"/>
@@ -2343,56 +2501,56 @@
       <c r="CU3"/>
       <c r="CV3"/>
       <c r="CW3" t="s">
-        <v>242</v>
+        <v>266</v>
       </c>
       <c r="CX3" t="s">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="CY3" t="s">
-        <v>244</v>
+        <v>268</v>
       </c>
       <c r="CZ3" t="s">
-        <v>245</v>
+        <v>269</v>
       </c>
       <c r="DA3" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="DB3" t="s">
-        <v>247</v>
+        <v>271</v>
       </c>
       <c r="DC3" t="s">
-        <v>248</v>
+        <v>272</v>
       </c>
       <c r="DD3" t="s">
-        <v>249</v>
+        <v>273</v>
       </c>
       <c r="DE3" t="s">
-        <v>250</v>
+        <v>274</v>
       </c>
       <c r="DF3" t="s">
-        <v>251</v>
+        <v>275</v>
       </c>
       <c r="DG3" t="s">
-        <v>252</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="E4"/>
       <c r="F4" t="s">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c r="G4" t="s">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -2402,242 +2560,242 @@
       <c r="M4"/>
       <c r="N4"/>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="P4" t="s">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c r="Q4" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="U4"/>
       <c r="V4" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="W4" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="X4" t="s">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c r="Y4" t="s">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c r="Z4"/>
       <c r="AA4" t="s">
-        <v>210</v>
+        <v>234</v>
       </c>
       <c r="AB4" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="AC4" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="AD4" t="s">
-        <v>212</v>
+        <v>236</v>
       </c>
       <c r="AE4"/>
       <c r="AF4" t="s">
-        <v>263</v>
+        <v>287</v>
       </c>
       <c r="AG4" t="s">
-        <v>264</v>
+        <v>288</v>
       </c>
       <c r="AH4" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="AI4" t="s">
-        <v>214</v>
+        <v>238</v>
       </c>
       <c r="AJ4" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="AK4"/>
       <c r="AL4" t="s">
-        <v>265</v>
+        <v>289</v>
       </c>
       <c r="AM4" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="AN4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="AO4"/>
       <c r="AP4" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="AQ4" t="s">
-        <v>267</v>
+        <v>291</v>
       </c>
       <c r="AR4"/>
       <c r="AS4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="AT4" t="s">
-        <v>268</v>
+        <v>292</v>
       </c>
       <c r="AU4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AV4" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="AW4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="AX4" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="AY4" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="AZ4" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="BA4" t="s">
-        <v>271</v>
+        <v>295</v>
       </c>
       <c r="BB4"/>
       <c r="BC4"/>
       <c r="BD4"/>
       <c r="BE4"/>
       <c r="BF4" t="s">
-        <v>272</v>
+        <v>296</v>
       </c>
       <c r="BG4"/>
       <c r="BH4" t="s">
-        <v>273</v>
+        <v>297</v>
       </c>
       <c r="BI4" t="s">
-        <v>274</v>
+        <v>298</v>
       </c>
       <c r="BJ4" t="s">
-        <v>275</v>
+        <v>299</v>
       </c>
       <c r="BK4" t="s">
-        <v>276</v>
+        <v>300</v>
       </c>
       <c r="BL4" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="BM4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="BN4" t="s">
-        <v>278</v>
+        <v>302</v>
       </c>
       <c r="BO4" t="s">
-        <v>279</v>
+        <v>303</v>
       </c>
       <c r="BP4"/>
       <c r="BQ4" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="BR4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="BS4" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="BT4"/>
       <c r="BU4"/>
       <c r="BV4"/>
       <c r="BW4" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="BX4" t="s">
-        <v>282</v>
+        <v>306</v>
       </c>
       <c r="BY4"/>
       <c r="BZ4" t="s">
-        <v>283</v>
+        <v>307</v>
       </c>
       <c r="CA4" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="CB4"/>
       <c r="CC4" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="CD4"/>
       <c r="CE4" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="CF4"/>
       <c r="CG4" t="s">
-        <v>236</v>
+        <v>260</v>
       </c>
       <c r="CH4" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
       <c r="CI4" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="CJ4" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="CK4" t="s">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="CL4" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
       <c r="CM4" t="s">
-        <v>291</v>
+        <v>315</v>
       </c>
       <c r="CN4" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="CO4" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="CP4" t="s">
-        <v>238</v>
+        <v>262</v>
       </c>
       <c r="CQ4" t="s">
-        <v>293</v>
+        <v>317</v>
       </c>
       <c r="CR4" t="s">
-        <v>294</v>
+        <v>318</v>
       </c>
       <c r="CS4" t="s">
-        <v>237</v>
+        <v>261</v>
       </c>
       <c r="CT4" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="CU4" t="s">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="CV4"/>
       <c r="CW4" t="s">
-        <v>296</v>
+        <v>320</v>
       </c>
       <c r="CX4" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="CY4" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="CZ4" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="DA4" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="DB4" t="s">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="DC4" t="s">
-        <v>302</v>
+        <v>326</v>
       </c>
       <c r="DD4" t="s">
-        <v>303</v>
+        <v>327</v>
       </c>
       <c r="DE4"/>
       <c r="DF4"/>

</xml_diff>